<commit_message>
Updated Professionalism Deliverables and and Work Process Spreadsheet
</commit_message>
<xml_diff>
--- a/Oswyn/Deliverables Tracking.xlsx
+++ b/Oswyn/Deliverables Tracking.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -128,18 +128,9 @@
     <t>Record Actual Hours</t>
   </si>
   <si>
-    <t>Review, Release, Version Control Check Lists</t>
-  </si>
-  <si>
-    <t>Task List Format</t>
-  </si>
-  <si>
     <t>Work Day Enumeration</t>
   </si>
   <si>
-    <t>Phase vs Guidence Level</t>
-  </si>
-  <si>
     <t>Project Scoping</t>
   </si>
   <si>
@@ -159,6 +150,27 @@
   </si>
   <si>
     <t>End fo Day</t>
+  </si>
+  <si>
+    <t>Release Check List</t>
+  </si>
+  <si>
+    <t>Version Control Check List</t>
+  </si>
+  <si>
+    <t>Error Mitigation Stratagy</t>
+  </si>
+  <si>
+    <t>Task List Template</t>
+  </si>
+  <si>
+    <t>Responsibility Guidelines</t>
+  </si>
+  <si>
+    <t>Review Check List</t>
+  </si>
+  <si>
+    <t>Conflict Guidelines</t>
   </si>
 </sst>
 </file>
@@ -674,13 +686,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="349">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1445,7 +1457,7 @@
       </c>
       <c r="D1" s="16"/>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18">
@@ -1453,11 +1465,11 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18">
@@ -1465,7 +1477,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16">
@@ -1498,8 +1510,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="16">
-      <c r="A6" s="23" t="s">
-        <v>42</v>
+      <c r="A6" s="22" t="s">
+        <v>39</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -1511,12 +1523,12 @@
       <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" ht="18">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1533,10 +1545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A7" sqref="A7:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1565,7 +1577,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" t="s">
@@ -1577,7 +1589,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" t="s">
@@ -1721,36 +1733,56 @@
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="24" t="s">
         <v>27</v>
       </c>
       <c r="E7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="30">
-      <c r="A9" s="22" t="s">
+    <row r="12" spans="1:19">
+      <c r="A12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="22" t="s">
+    <row r="13" spans="1:19">
+      <c r="A13" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1797,7 +1829,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" t="s">
@@ -1809,7 +1841,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" t="s">

</xml_diff>

<commit_message>
Added feedback and Updated Deliverables Status
</commit_message>
<xml_diff>
--- a/Oswyn/Deliverables Tracking.xlsx
+++ b/Oswyn/Deliverables Tracking.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="32940" yWindow="3600" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Standup" sheetId="3" r:id="rId1"/>
     <sheet name="Professionalism" sheetId="2" r:id="rId2"/>
     <sheet name="Hardware Development Process" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -286,7 +286,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="351">
+  <cellStyleXfs count="355">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -638,8 +638,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -701,8 +705,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="351">
+  <cellStyles count="355">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -878,6 +886,8 @@
     <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1053,6 +1063,8 @@
     <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1450,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView zoomScale="265" zoomScaleNormal="265" zoomScalePageLayoutView="265" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1461,28 +1473,28 @@
     <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16">
+    <row r="1" spans="1:10" ht="16">
       <c r="A1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18">
+    <row r="2" spans="1:10" ht="18">
       <c r="A2" s="21" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18">
+    <row r="3" spans="1:10" ht="18">
       <c r="A3" s="21" t="s">
         <v>28</v>
       </c>
@@ -1490,7 +1502,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16">
+    <row r="5" spans="1:10" ht="16">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
@@ -1498,32 +1510,35 @@
         <v>43003</v>
       </c>
       <c r="C5" s="13">
+        <v>43006</v>
+      </c>
+      <c r="D5" s="13">
         <v>43010</v>
       </c>
-      <c r="D5" s="13">
+      <c r="E5" s="13">
         <v>43017</v>
       </c>
-      <c r="E5" s="13">
+      <c r="F5" s="13">
         <v>43024</v>
       </c>
-      <c r="F5" s="13">
+      <c r="G5" s="13">
         <v>43031</v>
       </c>
-      <c r="G5" s="13">
+      <c r="H5" s="13">
         <v>43038</v>
       </c>
-      <c r="H5" s="13">
+      <c r="I5" s="13">
         <v>43045</v>
       </c>
-      <c r="I5" s="13">
+      <c r="J5" s="13">
         <v>43052</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16">
+    <row r="6" spans="1:10" ht="16">
       <c r="A6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="27" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="13"/>
@@ -1533,13 +1548,17 @@
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:9" ht="18">
+      <c r="J6" s="13"/>
+    </row>
+    <row r="7" spans="1:10" ht="18">
       <c r="A7" s="23" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="18">
+      <c r="C7" s="28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18">
       <c r="A8" s="23" t="s">
         <v>34</v>
       </c>
@@ -1560,7 +1579,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1748,7 +1767,7 @@
       <c r="A7" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="26" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1813,7 +1832,7 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2005,7 +2024,7 @@
         <v>33</v>
       </c>
       <c r="C7" s="10"/>
-      <c r="E7" t="s">
+      <c r="E7" s="25" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2014,7 +2033,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="10"/>
-      <c r="E8" t="s">
+      <c r="E8" s="26" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated incorrect assignment for deliverables tracking
</commit_message>
<xml_diff>
--- a/Oswyn/Deliverables Tracking.xlsx
+++ b/Oswyn/Deliverables Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="940" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="940" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Standup" sheetId="3" r:id="rId1"/>
@@ -695,7 +695,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -759,6 +759,7 @@
     <xf numFmtId="14" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="405">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1970,9 +1971,9 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="9340" topLeftCell="F1" activePane="topRight"/>
+      <pane xSplit="9340" topLeftCell="D1" activePane="topRight"/>
       <selection activeCell="A19" sqref="A19"/>
-      <selection pane="topRight" activeCell="I19" sqref="I19"/>
+      <selection pane="topRight" activeCell="F14" sqref="F14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2223,9 +2224,9 @@
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="3" t="s">

</xml_diff>

<commit_message>
Hardware Hours included in Task Enumeration
</commit_message>
<xml_diff>
--- a/Oswyn/Deliverables Tracking.xlsx
+++ b/Oswyn/Deliverables Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="940" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="940" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Standup" sheetId="3" r:id="rId1"/>
@@ -695,7 +695,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -759,6 +759,7 @@
     <xf numFmtId="14" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="405">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1970,9 +1971,9 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="9340" topLeftCell="F1" activePane="topRight"/>
+      <pane xSplit="9340" topLeftCell="D1" activePane="topRight"/>
       <selection activeCell="A19" sqref="A19"/>
-      <selection pane="topRight" activeCell="I19" sqref="I19"/>
+      <selection pane="topRight" activeCell="F14" sqref="F14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2223,9 +2224,9 @@
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="3" t="s">

</xml_diff>

<commit_message>
Updated Deliverables status 10/18
</commit_message>
<xml_diff>
--- a/Oswyn/Deliverables Tracking.xlsx
+++ b/Oswyn/Deliverables Tracking.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Flow Diagram</t>
   </si>
   <si>
-    <t>Record Actual Hours</t>
-  </si>
-  <si>
     <t>Work Day Enumeration</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>Oswyn</t>
   </si>
   <si>
-    <t>End fo Day</t>
-  </si>
-  <si>
     <t>Release Check List</t>
   </si>
   <si>
@@ -174,6 +168,9 @@
   </si>
   <si>
     <t>Sub Function Component Order</t>
+  </si>
+  <si>
+    <t>All Due End of Day</t>
   </si>
 </sst>
 </file>
@@ -183,7 +180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -230,11 +227,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -245,6 +237,33 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -288,7 +307,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="405">
+  <cellStyleXfs count="453">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -694,17 +713,62 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -747,21 +811,56 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="405">
+  <cellStyles count="453">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -964,6 +1063,30 @@
     <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1166,6 +1289,30 @@
     <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1565,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView zoomScale="265" zoomScaleNormal="265" zoomScalePageLayoutView="265" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="B1" zoomScale="265" zoomScaleNormal="265" zoomScalePageLayoutView="265" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1575,111 +1722,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="15"/>
+      <c r="E1" s="14"/>
       <c r="F1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18">
+      <c r="A2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:10" ht="18">
+      <c r="A3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" t="s">
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16">
+      <c r="A6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="11">
+        <v>43003</v>
+      </c>
+      <c r="C6" s="11">
+        <v>43006</v>
+      </c>
+      <c r="D6" s="11">
+        <v>43010</v>
+      </c>
+      <c r="E6" s="11">
+        <v>43017</v>
+      </c>
+      <c r="F6" s="11">
+        <v>43024</v>
+      </c>
+      <c r="G6" s="11">
+        <v>43031</v>
+      </c>
+      <c r="H6" s="11">
+        <v>43038</v>
+      </c>
+      <c r="I6" s="11">
+        <v>43045</v>
+      </c>
+      <c r="J6" s="11">
+        <v>43052</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16">
+      <c r="A7" s="20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="16">
-      <c r="A5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="12">
-        <v>43003</v>
-      </c>
-      <c r="C5" s="12">
-        <v>43006</v>
-      </c>
-      <c r="D5" s="12">
-        <v>43010</v>
-      </c>
-      <c r="E5" s="12">
-        <v>43017</v>
-      </c>
-      <c r="F5" s="12">
-        <v>43024</v>
-      </c>
-      <c r="G5" s="12">
-        <v>43031</v>
-      </c>
-      <c r="H5" s="12">
-        <v>43038</v>
-      </c>
-      <c r="I5" s="12">
-        <v>43045</v>
-      </c>
-      <c r="J5" s="12">
-        <v>43052</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16">
-      <c r="A6" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" ht="18">
-      <c r="A7" s="22" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" ht="18">
+      <c r="A8" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="18">
-      <c r="A8" s="22" t="s">
-        <v>27</v>
-      </c>
       <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1696,263 +1828,281 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
       <pane xSplit="8360" topLeftCell="E1" activePane="topRight"/>
-      <selection activeCell="A8" sqref="A8"/>
-      <selection pane="topRight" activeCell="J14" sqref="J14"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="topRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" style="28" customWidth="1"/>
+    <col min="2" max="2" width="12" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="28" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9" style="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9" style="28" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="8" style="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9" style="28" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="16">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" t="s">
+      <c r="D1" s="30"/>
+      <c r="E1" s="28" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="18">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="18">
+      <c r="A3" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="18">
-      <c r="A3" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" t="s">
+      <c r="D3" s="34"/>
+      <c r="E3" s="28" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="4"/>
-      <c r="C4" s="3"/>
+      <c r="A4" s="35"/>
+      <c r="C4" s="36"/>
     </row>
     <row r="5" spans="1:19" ht="16">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" s="28" t="str">
         <f>TEXT(C6,"ddd")</f>
         <v>Wed</v>
       </c>
-      <c r="D5" t="str">
+      <c r="D5" s="28" t="str">
         <f t="shared" ref="D5:S5" si="0">TEXT(D6,"ddd")</f>
         <v>Sat</v>
       </c>
-      <c r="E5" t="str">
+      <c r="E5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="F5" t="str">
+      <c r="F5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="G5" t="str">
+      <c r="G5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="H5" t="str">
+      <c r="H5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Sat</v>
       </c>
-      <c r="I5" t="str">
+      <c r="I5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="J5" t="str">
+      <c r="J5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="K5" t="str">
+      <c r="K5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="L5" t="str">
+      <c r="L5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Sat</v>
       </c>
-      <c r="M5" t="str">
+      <c r="M5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="N5" t="str">
+      <c r="N5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="O5" t="str">
+      <c r="O5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="P5" t="str">
+      <c r="P5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Sat</v>
       </c>
-      <c r="Q5" t="str">
+      <c r="Q5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="R5" t="str">
+      <c r="R5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="S5" t="str">
+      <c r="S5" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="1" customFormat="1" ht="16">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:19" s="40" customFormat="1" ht="16">
+      <c r="A6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="38">
         <v>42998</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="39">
         <v>43001</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="39">
         <v>43003</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="39">
         <v>43010</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="38">
         <v>43012</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="39">
         <v>43015</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="39">
         <v>43017</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="39">
         <v>43024</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="38">
         <v>43026</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="39">
         <v>43029</v>
       </c>
-      <c r="M6" s="12">
+      <c r="M6" s="39">
         <v>43031</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="39">
         <v>43038</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="38">
         <v>43040</v>
       </c>
-      <c r="P6" s="12">
+      <c r="P6" s="39">
         <v>43043</v>
       </c>
-      <c r="Q6" s="12">
+      <c r="Q6" s="39">
         <v>43045</v>
       </c>
-      <c r="R6" s="12">
+      <c r="R6" s="39">
         <v>43052</v>
       </c>
-      <c r="S6" s="14">
+      <c r="S6" s="38">
         <v>43055</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="23" t="s">
+    <row r="7" spans="1:19" ht="16" customHeight="1">
+      <c r="A7" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+    </row>
+    <row r="8" spans="1:19" ht="16">
+      <c r="A8" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="25"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="23" t="s">
+      <c r="I9" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="I8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="23" t="s">
+      <c r="I10" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="41"/>
+    </row>
+    <row r="13" spans="1:19" ht="16">
+      <c r="A13" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="I9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="23" t="s">
+      <c r="J13" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="30"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="I10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" t="s">
+      <c r="J14" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" s="43"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="28" t="s">
         <v>28</v>
-      </c>
-      <c r="J12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1970,17 +2120,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="9340" topLeftCell="D1" activePane="topRight"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <pane xSplit="9340" topLeftCell="C1" activePane="topRight"/>
       <selection activeCell="A19" sqref="A19"/>
-      <selection pane="topRight" activeCell="F14" sqref="F14:H14"/>
+      <selection pane="topRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="44.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
@@ -1990,54 +2140,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="16">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="24"/>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="18">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="15"/>
+        <v>32</v>
+      </c>
+      <c r="D2" s="14"/>
       <c r="E2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="18">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="16"/>
+        <v>33</v>
+      </c>
+      <c r="D3" s="15"/>
       <c r="E3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="D4" s="17"/>
+      <c r="D4" s="16"/>
       <c r="E4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="18">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:19" ht="16">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="5"/>
       <c r="C6" t="str">
         <f>TEXT(C7,"ddd")</f>
         <v>Wed</v>
@@ -2108,61 +2258,61 @@
       </c>
     </row>
     <row r="7" spans="1:19" s="1" customFormat="1" ht="16">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>42998</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>43001</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>43003</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>43010</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>43012</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>43015</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>43017</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="11">
         <v>43024</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="13">
         <v>43026</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="11">
         <v>43029</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="11">
         <v>43031</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="11">
         <v>43038</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O7" s="13">
         <v>43040</v>
       </c>
-      <c r="P7" s="12">
+      <c r="P7" s="11">
         <v>43043</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="Q7" s="11">
         <v>43045</v>
       </c>
-      <c r="R7" s="12">
+      <c r="R7" s="11">
         <v>43052</v>
       </c>
-      <c r="S7" s="14">
+      <c r="S7" s="13">
         <v>43055</v>
       </c>
     </row>
@@ -2170,170 +2320,175 @@
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="E8" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
+      <c r="C8" s="8"/>
+      <c r="E8" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:19" ht="16">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="E9" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
+      <c r="C9" s="8"/>
+      <c r="E9" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="C10" s="9"/>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:19" ht="16">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="16"/>
+      <c r="C11" s="9"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
+      <c r="C12" s="9"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
+      <c r="C13" s="9"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="I16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="I17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="9"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="10"/>
-      <c r="I18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="10"/>
-      <c r="I20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="C20" s="9"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="9"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="9"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="9"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="9"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="5" t="s">
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="9"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="C28" s="9"/>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="B27" s="4"/>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="9"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="9"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="C31" s="9"/>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="C31" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>